<commit_message>
日常更新：<update by home laptop x14 pro>
</commit_message>
<xml_diff>
--- a/00-doc/src/00_todo/00_todo.xlsx
+++ b/00-doc/src/00_todo/00_todo.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="208">
   <si>
     <t>month goals：
 1、oral practise everyday 
@@ -208,6 +208,10 @@
   </si>
   <si>
     <t>1、stare at stocks</t>
+  </si>
+  <si>
+    <t>1、stare at stocks
+2、waste in YouTube policy</t>
   </si>
   <si>
     <t>month goals：
@@ -4114,8 +4118,8 @@
   <sheetPr/>
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -4374,124 +4378,220 @@
       </c>
       <c r="F14" s="43"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" ht="84" spans="1:6">
       <c r="A15" s="20">
         <v>45609</v>
       </c>
-      <c r="B15" s="44"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
+      <c r="B15" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>20</v>
+      </c>
       <c r="F15" s="43"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" ht="84" spans="1:6">
       <c r="A16" s="20">
         <v>45610</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
+      <c r="B16" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="41" t="s">
+        <v>20</v>
+      </c>
       <c r="F16" s="43"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" ht="84" spans="1:6">
       <c r="A17" s="20">
         <v>45611</v>
       </c>
-      <c r="B17" s="44"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
+      <c r="B17" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>20</v>
+      </c>
       <c r="F17" s="41"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" ht="84" spans="1:6">
       <c r="A18" s="9">
         <v>45612</v>
       </c>
-      <c r="B18" s="44"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
+      <c r="B18" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="41" t="s">
+        <v>20</v>
+      </c>
       <c r="F18" s="41"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" ht="84" spans="1:6">
       <c r="A19" s="9">
         <v>45613</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
+      <c r="B19" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="41" t="s">
+        <v>20</v>
+      </c>
       <c r="F19" s="41"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" ht="84" spans="1:6">
       <c r="A20" s="20">
         <v>45614</v>
       </c>
-      <c r="B20" s="44"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
+      <c r="B20" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="41" t="s">
+        <v>20</v>
+      </c>
       <c r="F20" s="41"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" ht="84" spans="1:6">
       <c r="A21" s="20">
         <v>45615</v>
       </c>
-      <c r="B21" s="44"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
+      <c r="B21" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="41" t="s">
+        <v>20</v>
+      </c>
       <c r="F21" s="43"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" ht="84" spans="1:6">
       <c r="A22" s="20">
         <v>45616</v>
       </c>
-      <c r="B22" s="44"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
+      <c r="B22" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="41" t="s">
+        <v>20</v>
+      </c>
       <c r="F22" s="43"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" ht="84" spans="1:6">
       <c r="A23" s="20">
         <v>45617</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
+      <c r="B23" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="41" t="s">
+        <v>20</v>
+      </c>
       <c r="F23" s="43"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" ht="84" spans="1:6">
       <c r="A24" s="20">
         <v>45618</v>
       </c>
-      <c r="B24" s="44"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
+      <c r="B24" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="41" t="s">
+        <v>20</v>
+      </c>
       <c r="F24" s="43"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" ht="84" spans="1:6">
       <c r="A25" s="9">
         <v>45619</v>
       </c>
-      <c r="B25" s="44"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
+      <c r="B25" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="41" t="s">
+        <v>21</v>
+      </c>
       <c r="F25" s="43"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" ht="84" spans="1:6">
       <c r="A26" s="9">
         <v>45620</v>
       </c>
-      <c r="B26" s="44"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
+      <c r="B26" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="41" t="s">
+        <v>21</v>
+      </c>
       <c r="F26" s="43"/>
     </row>
     <row r="27" spans="1:6">
@@ -4641,7 +4741,7 @@
   <sheetData>
     <row r="1" ht="67" customHeight="1" spans="1:6">
       <c r="A1" s="24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -4674,16 +4774,16 @@
         <v>45566</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F3" s="11"/>
     </row>
@@ -4692,19 +4792,19 @@
         <v>45567</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" ht="70" spans="1:6">
@@ -4715,13 +4815,13 @@
         <v>7</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F5" s="11"/>
     </row>
@@ -4733,13 +4833,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F6" s="8"/>
     </row>
@@ -4751,13 +4851,13 @@
         <v>7</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F7" s="8"/>
     </row>
@@ -4769,13 +4869,13 @@
         <v>7</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F8" s="8"/>
     </row>
@@ -4787,10 +4887,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="8"/>
@@ -4803,10 +4903,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="8"/>
@@ -4819,10 +4919,10 @@
         <v>7</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="8"/>
@@ -4835,10 +4935,10 @@
         <v>7</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="8"/>
@@ -4851,13 +4951,13 @@
         <v>7</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F13" s="8"/>
     </row>
@@ -4869,13 +4969,13 @@
         <v>7</v>
       </c>
       <c r="C14" s="38" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F14" s="8"/>
     </row>
@@ -4887,13 +4987,13 @@
         <v>7</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F15" s="8"/>
     </row>
@@ -4905,13 +5005,13 @@
         <v>7</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F16" s="8"/>
     </row>
@@ -4923,10 +5023,10 @@
         <v>7</v>
       </c>
       <c r="C17" s="36" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>16</v>
@@ -4941,13 +5041,13 @@
         <v>7</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F18" s="11"/>
     </row>
@@ -4959,13 +5059,13 @@
         <v>7</v>
       </c>
       <c r="C19" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="33" t="s">
-        <v>63</v>
-      </c>
       <c r="E19" s="11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F19" s="11"/>
     </row>
@@ -4977,13 +5077,13 @@
         <v>7</v>
       </c>
       <c r="C20" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="33" t="s">
-        <v>63</v>
-      </c>
       <c r="E20" s="11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F20" s="11"/>
     </row>
@@ -4995,13 +5095,13 @@
         <v>7</v>
       </c>
       <c r="C21" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="33" t="s">
-        <v>63</v>
-      </c>
       <c r="E21" s="11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F21" s="8"/>
     </row>
@@ -5013,13 +5113,13 @@
         <v>7</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D22" s="33" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F22" s="8"/>
     </row>
@@ -5031,13 +5131,13 @@
         <v>7</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D23" s="33" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F23" s="8"/>
     </row>
@@ -5049,13 +5149,13 @@
         <v>7</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D24" s="33" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F24" s="8"/>
     </row>
@@ -5067,13 +5167,13 @@
         <v>7</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D25" s="33" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F25" s="8"/>
     </row>
@@ -5085,13 +5185,13 @@
         <v>7</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D26" s="33" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F26" s="8"/>
     </row>
@@ -5103,13 +5203,13 @@
         <v>7</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D27" s="33" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F27" s="8"/>
     </row>
@@ -5121,13 +5221,13 @@
         <v>7</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D28" s="33" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F28" s="8"/>
     </row>
@@ -5139,13 +5239,13 @@
         <v>7</v>
       </c>
       <c r="C29" s="38" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D29" s="33" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F29" s="8"/>
     </row>
@@ -5157,13 +5257,13 @@
         <v>7</v>
       </c>
       <c r="C30" s="38" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D30" s="33" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F30" s="8"/>
     </row>
@@ -5175,13 +5275,13 @@
         <v>7</v>
       </c>
       <c r="C31" s="38" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D31" s="33" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F31" s="8"/>
     </row>
@@ -5193,13 +5293,13 @@
         <v>7</v>
       </c>
       <c r="C32" s="36" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D32" s="33" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F32" s="8"/>
     </row>
@@ -5211,13 +5311,13 @@
         <v>7</v>
       </c>
       <c r="C33" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D33" s="33" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F33" s="14"/>
     </row>
@@ -5229,19 +5329,19 @@
         <v>7</v>
       </c>
       <c r="C34" s="38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D34" s="33" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F34" s="14"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B35" s="14"/>
       <c r="C35" s="14"/>
@@ -5328,7 +5428,7 @@
   <sheetData>
     <row r="1" ht="67" customHeight="1" spans="1:6">
       <c r="A1" s="24" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -5364,10 +5464,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>10</v>
@@ -5382,10 +5482,10 @@
         <v>7</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>10</v>
@@ -5400,13 +5500,13 @@
         <v>7</v>
       </c>
       <c r="C5" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="35" t="s">
-        <v>78</v>
-      </c>
       <c r="E5" s="11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F5" s="11"/>
     </row>
@@ -5418,16 +5518,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="35" t="s">
         <v>79</v>
-      </c>
-      <c r="D6" s="35" t="s">
-        <v>78</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" ht="56" spans="1:6">
@@ -5438,16 +5538,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="35" t="s">
         <v>79</v>
-      </c>
-      <c r="D7" s="35" t="s">
-        <v>78</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" ht="56" spans="1:6">
@@ -5458,16 +5558,16 @@
         <v>7</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D8" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="9" ht="70" spans="1:6">
@@ -5475,19 +5575,19 @@
         <v>45542</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" ht="70" spans="1:6">
@@ -5498,16 +5598,16 @@
         <v>7</v>
       </c>
       <c r="C10" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>87</v>
-      </c>
-      <c r="D10" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="11" ht="56" spans="1:6">
@@ -5518,16 +5618,16 @@
         <v>7</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" ht="56" spans="1:6">
@@ -5538,16 +5638,16 @@
         <v>7</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" ht="56" spans="1:6">
@@ -5558,16 +5658,16 @@
         <v>7</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" ht="56" spans="1:6">
@@ -5578,16 +5678,16 @@
         <v>7</v>
       </c>
       <c r="C14" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="8" t="s">
         <v>94</v>
-      </c>
-      <c r="D14" s="35" t="s">
-        <v>95</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="15" ht="56" spans="1:6">
@@ -5595,16 +5695,16 @@
         <v>45548</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F15" s="8"/>
     </row>
@@ -5616,13 +5716,13 @@
         <v>7</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F16" s="8"/>
     </row>
@@ -5634,13 +5734,13 @@
         <v>7</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F17" s="11"/>
     </row>
@@ -5652,13 +5752,13 @@
         <v>7</v>
       </c>
       <c r="C18" s="36" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F18" s="11"/>
     </row>
@@ -5670,10 +5770,10 @@
         <v>7</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>10</v>
@@ -5685,16 +5785,16 @@
         <v>45553</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C20" s="38" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F20" s="11"/>
     </row>
@@ -5703,16 +5803,16 @@
         <v>45554</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F21" s="8"/>
     </row>
@@ -5721,16 +5821,16 @@
         <v>45555</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D22" s="33" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F22" s="8"/>
     </row>
@@ -5739,16 +5839,16 @@
         <v>45556</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C23" s="36" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D23" s="33" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F23" s="8"/>
     </row>
@@ -5760,13 +5860,13 @@
         <v>7</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D24" s="33" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F24" s="8"/>
     </row>
@@ -5778,10 +5878,10 @@
         <v>7</v>
       </c>
       <c r="C25" s="36" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D25" s="33" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>10</v>
@@ -5796,10 +5896,10 @@
         <v>7</v>
       </c>
       <c r="C26" s="36" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D26" s="35" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>10</v>
@@ -5814,10 +5914,10 @@
         <v>7</v>
       </c>
       <c r="C27" s="36" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D27" s="35" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>10</v>
@@ -5832,13 +5932,13 @@
         <v>7</v>
       </c>
       <c r="C28" s="36" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D28" s="35" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F28" s="8"/>
     </row>
@@ -5850,10 +5950,10 @@
         <v>7</v>
       </c>
       <c r="C29" s="36" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D29" s="35" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E29" s="11" t="s">
         <v>10</v>
@@ -5868,13 +5968,13 @@
         <v>7</v>
       </c>
       <c r="C30" s="36" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D30" s="35" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F30" s="8"/>
     </row>
@@ -5886,13 +5986,13 @@
         <v>7</v>
       </c>
       <c r="C31" s="36" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D31" s="35" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F31" s="8"/>
     </row>
@@ -5904,10 +6004,10 @@
         <v>7</v>
       </c>
       <c r="C32" s="36" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D32" s="35" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>10</v>
@@ -6001,7 +6101,7 @@
   <sheetData>
     <row r="1" ht="67" customHeight="1" spans="1:6">
       <c r="A1" s="24" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -6043,10 +6143,10 @@
         <v>0</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -6063,10 +6163,10 @@
         <v>1</v>
       </c>
       <c r="E4" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>137</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="5" ht="28" spans="1:6">
@@ -6083,10 +6183,10 @@
         <v>1</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -6103,10 +6203,10 @@
         <v>1</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -6124,7 +6224,7 @@
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -6142,7 +6242,7 @@
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="8" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -6159,10 +6259,10 @@
         <v>1</v>
       </c>
       <c r="E9" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>142</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -6180,7 +6280,7 @@
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -6198,7 +6298,7 @@
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" ht="28" spans="1:6">
@@ -6215,10 +6315,10 @@
         <v>1</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" ht="42" spans="1:6">
@@ -6235,10 +6335,10 @@
         <v>1</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" ht="42" spans="1:6">
@@ -6255,10 +6355,10 @@
         <v>1</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" ht="42" spans="1:6">
@@ -6275,10 +6375,10 @@
         <v>0</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" ht="42" spans="1:6">
@@ -6298,7 +6398,7 @@
         <v>10</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" ht="42" spans="1:6">
@@ -6318,7 +6418,7 @@
         <v>10</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" ht="42" spans="1:6">
@@ -6338,7 +6438,7 @@
         <v>10</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" ht="42" spans="1:6">
@@ -6355,10 +6455,10 @@
         <v>0</v>
       </c>
       <c r="E19" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="F19" s="11" t="s">
         <v>148</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="20" ht="42" spans="1:6">
@@ -6375,10 +6475,10 @@
         <v>0</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" ht="42" spans="1:6">
@@ -6395,10 +6495,10 @@
         <v>0</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" ht="42" spans="1:6">
@@ -6415,10 +6515,10 @@
         <v>0</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" ht="42" spans="1:6">
@@ -6438,7 +6538,7 @@
         <v>10</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" ht="42" spans="1:6">
@@ -6458,7 +6558,7 @@
         <v>10</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" ht="42" spans="1:6">
@@ -6478,7 +6578,7 @@
         <v>10</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" ht="42" spans="1:6">
@@ -6495,10 +6595,10 @@
         <v>0</v>
       </c>
       <c r="E26" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="F26" s="8" t="s">
         <v>152</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="27" ht="42" spans="1:6">
@@ -6515,7 +6615,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F27" s="8"/>
     </row>
@@ -6533,7 +6633,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F28" s="8"/>
     </row>
@@ -6551,7 +6651,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F29" s="8"/>
     </row>
@@ -6569,7 +6669,7 @@
         <v>0</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F30" s="8"/>
     </row>
@@ -6587,7 +6687,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F31" s="8"/>
     </row>
@@ -6605,7 +6705,7 @@
         <v>0</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F32" s="8"/>
     </row>
@@ -6623,13 +6723,13 @@
         <v>0</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="14" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
@@ -6718,7 +6818,7 @@
   <sheetData>
     <row r="1" ht="67" customHeight="1" spans="1:8">
       <c r="A1" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -6730,22 +6830,22 @@
     </row>
     <row r="2" ht="63" customHeight="1" spans="1:8">
       <c r="A2" s="15" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G2" s="19" t="s">
         <v>5</v>
@@ -6862,7 +6962,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H7" s="8"/>
     </row>
@@ -6886,7 +6986,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H8" s="8"/>
     </row>
@@ -6954,7 +7054,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H11" s="10"/>
     </row>
@@ -7000,7 +7100,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H13" s="8"/>
     </row>
@@ -7024,7 +7124,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H14" s="8"/>
     </row>
@@ -7048,7 +7148,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H15" s="8"/>
     </row>
@@ -7072,7 +7172,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H16" s="8"/>
     </row>
@@ -7118,7 +7218,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H18" s="8"/>
     </row>
@@ -7186,7 +7286,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H21" s="8"/>
     </row>
@@ -7210,7 +7310,7 @@
         <v>0</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H22" s="8"/>
     </row>
@@ -7234,7 +7334,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H23" s="8"/>
     </row>
@@ -7279,7 +7379,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H25" s="8"/>
     </row>
@@ -7303,7 +7403,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H26" s="8"/>
     </row>
@@ -7327,7 +7427,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H27" s="8"/>
     </row>
@@ -7348,7 +7448,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
@@ -7370,10 +7470,10 @@
         <v>1</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H29" s="8"/>
     </row>
@@ -7394,7 +7494,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
@@ -7477,7 +7577,7 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="14" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B35" s="14"/>
       <c r="C35" s="14"/>
@@ -7572,7 +7672,7 @@
   <sheetData>
     <row r="1" ht="48" customHeight="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -7582,16 +7682,16 @@
     </row>
     <row r="2" ht="63" customHeight="1" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>5</v>
@@ -7685,15 +7785,15 @@
         <v>45452</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -7701,10 +7801,10 @@
         <v>45453</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -7715,14 +7815,14 @@
         <v>45454</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F13" s="8"/>
     </row>
@@ -7731,14 +7831,14 @@
         <v>45455</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F14" s="8"/>
     </row>
@@ -7747,14 +7847,14 @@
         <v>45456</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F15" s="8"/>
     </row>
@@ -7763,14 +7863,14 @@
         <v>45457</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="11" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F16" s="8"/>
     </row>
@@ -7779,17 +7879,17 @@
         <v>45458</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="11" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" ht="42" spans="1:6">
@@ -7797,14 +7897,14 @@
         <v>45459</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="11" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F18" s="8"/>
     </row>
@@ -7813,14 +7913,14 @@
         <v>45460</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="11" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F19" s="8"/>
     </row>
@@ -7829,10 +7929,10 @@
         <v>45461</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
@@ -7843,14 +7943,14 @@
         <v>45462</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="11" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F21" s="8"/>
     </row>
@@ -7859,14 +7959,14 @@
         <v>45463</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="11" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F22" s="8"/>
     </row>
@@ -7875,14 +7975,14 @@
         <v>45464</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="11" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F23" s="8"/>
     </row>
@@ -7891,16 +7991,16 @@
         <v>45465</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D24" s="11">
         <v>2</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F24" s="8"/>
     </row>
@@ -7921,14 +8021,14 @@
         <v>45467</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="8" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F26" s="8"/>
     </row>
@@ -7937,10 +8037,10 @@
         <v>45468</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D27" s="8">
         <v>2</v>
@@ -7953,10 +8053,10 @@
         <v>45469</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D28" s="8">
         <v>1</v>
@@ -7969,10 +8069,10 @@
         <v>45470</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D29" s="8">
         <v>1</v>
@@ -7985,10 +8085,10 @@
         <v>45471</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
@@ -8002,11 +8102,11 @@
         <v>0.354166666666667</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="8" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F31" s="8"/>
     </row>
@@ -8018,19 +8118,19 @@
         <v>0.354166666666667</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D32" s="8">
         <v>1</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F32" s="8"/>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="14" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>

</xml_diff>